<commit_message>
Aktuelle Zahlen Stand Dez. 2019
</commit_message>
<xml_diff>
--- a/index/kreise-index-pop.xlsx
+++ b/index/kreise-index-pop.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\R\projekte\covid-19\index\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AEFF81-869A-4412-BBD2-5A8BF0CB4515}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -13,6 +19,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={630CD8DE-C7C6-43F5-B0DA-8DF855577D0C}</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{630CD8DE-C7C6-43F5-B0DA-8DF855577D0C}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Bevölkerungsstatistik Hessen zum 31.12.2019, https://statistik.hessen.de/sites/statistik.hessen.de/files/AI6_j19.pdf</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
@@ -286,8 +310,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="###\ ###\ ##0\ ;\–###\ ##0\ ;\—\ ;@\ \ "/>
+    <numFmt numFmtId="165" formatCode="#0.0\ ;\-#\ 0.0\ "/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -295,13 +325,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -313,18 +377,48 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard 2 2 2" xfId="3" xr:uid="{87A41CA5-1515-418A-8AF2-DD9AF8B49EA1}"/>
+    <cellStyle name="Standard 3" xfId="4" xr:uid="{2E24603D-4C08-4BB4-A724-7238C4C37233}"/>
+    <cellStyle name="Standard_2000" xfId="2" xr:uid="{F637BFF5-A148-41A1-9CBF-A8B73C017A93}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Jan Eggers" id="{C783D3D0-874A-44B7-8A5B-A185EDBE042E}" userId="S::Jan.Eggers@hr.de::65018185-ecc0-43b6-8af5-ebdb423a1ab7" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -604,20 +698,30 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A1" dT="2020-07-06T09:22:31.87" personId="{C783D3D0-874A-44B7-8A5B-A185EDBE042E}" id="{630CD8DE-C7C6-43F5-B0DA-8DF855577D0C}">
+    <text>Bevölkerungsstatistik Hessen zum 31.12.2019, https://statistik.hessen.de/sites/statistik.hessen.de/files/AI6_j19.pdf</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:S30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="7"/>
+    <col min="19" max="19" width="11.140625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +740,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -652,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -671,8 +775,8 @@
       <c r="F2">
         <v>49.641185</v>
       </c>
-      <c r="G2">
-        <v>269694</v>
+      <c r="G2" s="8">
+        <v>270340</v>
       </c>
       <c r="H2">
         <v>14697</v>
@@ -686,8 +790,14 @@
       <c r="K2">
         <v>59864</v>
       </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="N2" s="1"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="6"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -706,8 +816,8 @@
       <c r="F3">
         <v>49.872238000000003</v>
       </c>
-      <c r="G3">
-        <v>159207</v>
+      <c r="G3" s="8">
+        <v>159878</v>
       </c>
       <c r="H3">
         <v>9328</v>
@@ -721,8 +831,14 @@
       <c r="K3">
         <v>27416</v>
       </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="N3" s="4"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="6"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -741,8 +857,8 @@
       <c r="F4">
         <v>49.899272000000003</v>
       </c>
-      <c r="G4">
-        <v>297399</v>
+      <c r="G4" s="8">
+        <v>297844</v>
       </c>
       <c r="H4">
         <v>17252</v>
@@ -756,8 +872,14 @@
       <c r="K4">
         <v>61708</v>
       </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="N4" s="4"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="6"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>88</v>
       </c>
@@ -776,8 +898,8 @@
       <c r="F5">
         <v>50.110880000000002</v>
       </c>
-      <c r="G5">
-        <v>753056</v>
+      <c r="G5" s="8">
+        <v>763380</v>
       </c>
       <c r="H5">
         <v>48954</v>
@@ -791,8 +913,14 @@
       <c r="K5">
         <v>117760</v>
       </c>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="N5" s="4"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="6"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -811,8 +939,8 @@
       <c r="F6">
         <v>50.553229999999999</v>
       </c>
-      <c r="G6">
-        <v>222584</v>
+      <c r="G6" s="8">
+        <v>223145</v>
       </c>
       <c r="H6">
         <v>12557</v>
@@ -826,8 +954,14 @@
       <c r="K6">
         <v>46895</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="N6" s="4"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="6"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -846,8 +980,8 @@
       <c r="F7">
         <v>50.586194999999996</v>
       </c>
-      <c r="G7">
-        <v>268876</v>
+      <c r="G7" s="8">
+        <v>270688</v>
       </c>
       <c r="H7">
         <v>14778</v>
@@ -861,8 +995,14 @@
       <c r="K7">
         <v>52052</v>
       </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="N7" s="4"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="6"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -881,8 +1021,8 @@
       <c r="F8">
         <v>49.921619999999997</v>
       </c>
-      <c r="G8">
-        <v>274526</v>
+      <c r="G8" s="8">
+        <v>275726</v>
       </c>
       <c r="H8">
         <v>17378</v>
@@ -896,8 +1036,14 @@
       <c r="K8">
         <v>52778</v>
       </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="N8" s="4"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="6"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>31</v>
       </c>
@@ -916,8 +1062,8 @@
       <c r="F9">
         <v>50.867804999999997</v>
       </c>
-      <c r="G9">
-        <v>120829</v>
+      <c r="G9" s="8">
+        <v>120719</v>
       </c>
       <c r="H9">
         <v>6323</v>
@@ -931,8 +1077,14 @@
       <c r="K9">
         <v>28963</v>
       </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="N9" s="4"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>34</v>
       </c>
@@ -951,8 +1103,8 @@
       <c r="F10">
         <v>50.228406</v>
       </c>
-      <c r="G10">
-        <v>236564</v>
+      <c r="G10" s="8">
+        <v>236914</v>
       </c>
       <c r="H10">
         <v>13409</v>
@@ -966,8 +1118,14 @@
       <c r="K10">
         <v>53418</v>
       </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="N10" s="4"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -986,8 +1144,8 @@
       <c r="F11">
         <v>51.494179000000003</v>
       </c>
-      <c r="G11">
-        <v>236633</v>
+      <c r="G11" s="8">
+        <v>236764</v>
       </c>
       <c r="H11">
         <v>12213</v>
@@ -1001,8 +1159,14 @@
       <c r="K11">
         <v>58798</v>
       </c>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="N11" s="4"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>40</v>
       </c>
@@ -1021,8 +1185,8 @@
       <c r="F12">
         <v>51.314684</v>
       </c>
-      <c r="G12">
-        <v>201585</v>
+      <c r="G12" s="8">
+        <v>202137</v>
       </c>
       <c r="H12">
         <v>11651</v>
@@ -1036,8 +1200,14 @@
       <c r="K12">
         <v>39287</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="N12" s="4"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>43</v>
       </c>
@@ -1056,8 +1226,8 @@
       <c r="F13">
         <v>50.554439000000002</v>
       </c>
-      <c r="G13">
-        <v>253777</v>
+      <c r="G13" s="8">
+        <v>253319</v>
       </c>
       <c r="H13">
         <v>13858</v>
@@ -1071,8 +1241,14 @@
       <c r="K13">
         <v>56046</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="N13" s="4"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="6"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -1091,8 +1267,8 @@
       <c r="F14">
         <v>50.387253999999999</v>
       </c>
-      <c r="G14">
-        <v>172083</v>
+      <c r="G14" s="8">
+        <v>171912</v>
       </c>
       <c r="H14">
         <v>9144</v>
@@ -1106,8 +1282,14 @@
       <c r="K14">
         <v>36910</v>
       </c>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="N14" s="4"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="2"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="6"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>49</v>
       </c>
@@ -1126,8 +1308,8 @@
       <c r="F15">
         <v>50.203102999999999</v>
       </c>
-      <c r="G15">
-        <v>418950</v>
+      <c r="G15" s="8">
+        <v>420552</v>
       </c>
       <c r="H15">
         <v>23662</v>
@@ -1141,8 +1323,14 @@
       <c r="K15">
         <v>90193</v>
       </c>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="N15" s="4"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+      <c r="Q15" s="2"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="6"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1161,8 +1349,8 @@
       <c r="F16">
         <v>50.088576000000003</v>
       </c>
-      <c r="G16">
-        <v>237735</v>
+      <c r="G16" s="8">
+        <v>238558</v>
       </c>
       <c r="H16">
         <v>14218</v>
@@ -1176,8 +1364,14 @@
       <c r="K16">
         <v>50302</v>
       </c>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="N16" s="1"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="2"/>
+      <c r="Q16" s="2"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="6"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -1196,8 +1390,8 @@
       <c r="F17">
         <v>50.809004000000002</v>
       </c>
-      <c r="G17">
-        <v>246648</v>
+      <c r="G17" s="8">
+        <v>247084</v>
       </c>
       <c r="H17">
         <v>12898</v>
@@ -1211,8 +1405,14 @@
       <c r="K17">
         <v>48437</v>
       </c>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="N17" s="4"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2"/>
+      <c r="Q17" s="2"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="6"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -1231,8 +1431,8 @@
       <c r="F18">
         <v>49.657653000000003</v>
       </c>
-      <c r="G18">
-        <v>96798</v>
+      <c r="G18" s="8">
+        <v>96703</v>
       </c>
       <c r="H18">
         <v>4939</v>
@@ -1246,8 +1446,14 @@
       <c r="K18">
         <v>22823</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="N18" s="4"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="2"/>
+      <c r="Q18" s="2"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="6"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>61</v>
       </c>
@@ -1266,8 +1472,8 @@
       <c r="F19">
         <v>50.008938999999998</v>
       </c>
-      <c r="G19">
-        <v>354092</v>
+      <c r="G19" s="8">
+        <v>355813</v>
       </c>
       <c r="H19">
         <v>21213</v>
@@ -1281,8 +1487,14 @@
       <c r="K19">
         <v>75017</v>
       </c>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="N19" s="4"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="6"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>64</v>
       </c>
@@ -1301,8 +1513,8 @@
       <c r="F20">
         <v>50.100566999999998</v>
       </c>
-      <c r="G20">
-        <v>128744</v>
+      <c r="G20" s="8">
+        <v>130280</v>
       </c>
       <c r="H20">
         <v>8783</v>
@@ -1316,8 +1528,14 @@
       <c r="K20">
         <v>21186</v>
       </c>
-    </row>
-    <row r="21" spans="1:11">
+      <c r="N20" s="4"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="6"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>67</v>
       </c>
@@ -1336,8 +1554,8 @@
       <c r="F21">
         <v>50.140276</v>
       </c>
-      <c r="G21">
-        <v>187157</v>
+      <c r="G21" s="8">
+        <v>187160</v>
       </c>
       <c r="H21">
         <v>9792</v>
@@ -1351,8 +1569,14 @@
       <c r="K21">
         <v>42767</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="N21" s="4"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="6"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>70</v>
       </c>
@@ -1371,8 +1595,8 @@
       <c r="F22">
         <v>51.130940000000002</v>
       </c>
-      <c r="G22">
-        <v>180222</v>
+      <c r="G22" s="8">
+        <v>179673</v>
       </c>
       <c r="H22">
         <v>9103</v>
@@ -1386,8 +1610,14 @@
       <c r="K22">
         <v>41908</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="N22" s="4"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="6"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>73</v>
       </c>
@@ -1406,8 +1636,8 @@
       <c r="F23">
         <v>50.635728999999998</v>
       </c>
-      <c r="G23">
-        <v>105878</v>
+      <c r="G23" s="8">
+        <v>105643</v>
       </c>
       <c r="H23">
         <v>5017</v>
@@ -1421,8 +1651,14 @@
       <c r="K23">
         <v>25752</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="N23" s="1"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="6"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>76</v>
       </c>
@@ -1441,8 +1677,8 @@
       <c r="F24">
         <v>51.271859999999997</v>
       </c>
-      <c r="G24">
-        <v>156953</v>
+      <c r="G24" s="8">
+        <v>156406</v>
       </c>
       <c r="H24">
         <v>8178</v>
@@ -1456,8 +1692,14 @@
       <c r="K24">
         <v>36306</v>
       </c>
-    </row>
-    <row r="25" spans="1:11">
+      <c r="N24" s="4"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="6"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>79</v>
       </c>
@@ -1476,8 +1718,8 @@
       <c r="F25">
         <v>51.185803999999997</v>
       </c>
-      <c r="G25">
-        <v>101017</v>
+      <c r="G25" s="8">
+        <v>100629</v>
       </c>
       <c r="H25">
         <v>4864</v>
@@ -1491,8 +1733,14 @@
       <c r="K25">
         <v>25828</v>
       </c>
-    </row>
-    <row r="26" spans="1:11">
+      <c r="N25" s="4"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>82</v>
       </c>
@@ -1511,8 +1759,8 @@
       <c r="F26">
         <v>50.337760000000003</v>
       </c>
-      <c r="G26">
-        <v>306460</v>
+      <c r="G26" s="8">
+        <v>308339</v>
       </c>
       <c r="H26">
         <v>16941</v>
@@ -1526,8 +1774,14 @@
       <c r="K26">
         <v>64728</v>
       </c>
-    </row>
-    <row r="27" spans="1:11">
+      <c r="N26" s="4"/>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2"/>
+      <c r="Q26" s="2"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>85</v>
       </c>
@@ -1546,8 +1800,8 @@
       <c r="F27">
         <v>50.081698000000003</v>
       </c>
-      <c r="G27">
-        <v>278342</v>
+      <c r="G27" s="8">
+        <v>278474</v>
       </c>
       <c r="H27">
         <v>17824</v>
@@ -1561,9 +1815,40 @@
       <c r="K27">
         <v>55604</v>
       </c>
+      <c r="N27" s="4"/>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2"/>
+      <c r="Q27" s="2"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="6"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N28" s="4"/>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2"/>
+      <c r="Q28" s="2"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="6"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N29" s="4"/>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2"/>
+      <c r="Q29" s="2"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N30" s="4"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anpassung an Bevölkerungszahlen und Boosterimpfungen
</commit_message>
<xml_diff>
--- a/index/kreise-index-pop.xlsx
+++ b/index/kreise-index-pop.xlsx
@@ -1,18 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <extLst>
+    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
   <si>
     <t xml:space="preserve">kreis</t>
   </si>
@@ -119,7 +127,7 @@
     <t xml:space="preserve">Groß-Gerau, Stadt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.kreisgg.de/gesundheit/infektionsschutz/corona-krise-info-und-hotlines/</t>
+    <t xml:space="preserve">https://www.kreisgg.de/gesundheit/corona-krise-info-und-hotlines/</t>
   </si>
   <si>
     <t xml:space="preserve">Hochtaunuskreis</t>
@@ -350,15 +358,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="General"/>
+  </numFmts>
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -370,7 +395,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -378,1008 +403,773 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2" s="0" t="n">
         <v>8.653838</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2" s="0" t="n">
         <v>49.872238</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2" s="0" t="n">
         <v>159174</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="n">
+      <c r="E3" s="0" t="n">
         <v>8.682433</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3" s="0" t="n">
         <v>50.11088</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" s="0" t="n">
         <v>764104</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" s="0" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E4" t="n">
+      <c r="E4" s="0" t="n">
         <v>8.784442</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4" s="0" t="n">
         <v>50.100567</v>
       </c>
-      <c r="G4" t="n">
+      <c r="G4" s="0" t="n">
         <v>130892</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="0" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="0" t="n">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E5" s="0" t="n">
         <v>8.239138</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F5" s="0" t="n">
         <v>50.081698</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G5" s="0" t="n">
         <v>278609</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="0" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E6" t="n">
+      <c r="E6" s="0" t="n">
         <v>8.644017</v>
       </c>
-      <c r="F6" t="n">
+      <c r="F6" s="0" t="n">
         <v>49.641185</v>
       </c>
-      <c r="G6" t="n">
+      <c r="G6" s="0" t="n">
         <v>271015</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="0" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7" s="0" t="n">
         <v>8.840041</v>
       </c>
-      <c r="F7" t="n">
+      <c r="F7" s="0" t="n">
         <v>49.899272</v>
       </c>
-      <c r="G7" t="n">
+      <c r="G7" s="0" t="n">
         <v>297701</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="0" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E8" t="n">
+      <c r="E8" s="0" t="n">
         <v>8.482423</v>
       </c>
-      <c r="F8" t="n">
+      <c r="F8" s="0" t="n">
         <v>49.92162</v>
       </c>
-      <c r="G8" t="n">
+      <c r="G8" s="0" t="n">
         <v>275807</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="0" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E9" s="0" t="n">
         <v>8.61299</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F9" s="0" t="n">
         <v>50.228406</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G9" s="0" t="n">
         <v>237281</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="0" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
         <v>40</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="E10" t="n">
+      <c r="E10" s="0" t="n">
         <v>9.191488</v>
       </c>
-      <c r="F10" t="n">
+      <c r="F10" s="0" t="n">
         <v>50.203103</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" s="0" t="n">
         <v>421689</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H10" s="0" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E11" t="n">
+      <c r="E11" s="0" t="n">
         <v>8.446053</v>
       </c>
-      <c r="F11" t="n">
+      <c r="F11" s="0" t="n">
         <v>50.088576</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" s="0" t="n">
         <v>239264</v>
       </c>
-      <c r="H11" t="s">
+      <c r="H11" s="0" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="0" t="s">
         <v>49</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="E12" t="n">
+      <c r="E12" s="0" t="n">
         <v>8.99268</v>
       </c>
-      <c r="F12" t="n">
+      <c r="F12" s="0" t="n">
         <v>49.657653</v>
       </c>
-      <c r="G12" t="n">
+      <c r="G12" s="0" t="n">
         <v>96754</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" s="0" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="s">
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="E13" t="n">
+      <c r="E13" s="0" t="n">
         <v>8.781779</v>
       </c>
-      <c r="F13" t="n">
+      <c r="F13" s="0" t="n">
         <v>50.008939</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" s="0" t="n">
         <v>356542</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" s="0" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="s">
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="E14" t="n">
+      <c r="E14" s="0" t="n">
         <v>8.069825</v>
       </c>
-      <c r="F14" t="n">
+      <c r="F14" s="0" t="n">
         <v>50.140276</v>
       </c>
-      <c r="G14" t="n">
+      <c r="G14" s="0" t="n">
         <v>187433</v>
       </c>
-      <c r="H14" t="s">
+      <c r="H14" s="0" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15" s="0" t="n">
         <v>25</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="E15" t="n">
+      <c r="E15" s="0" t="n">
         <v>8.754091</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F15" s="0" t="n">
         <v>50.33776</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G15" s="0" t="n">
         <v>310353</v>
       </c>
-      <c r="H15" t="s">
+      <c r="H15" s="0" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="s">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="0" t="s">
         <v>66</v>
       </c>
-      <c r="E16" t="n">
+      <c r="E16" s="0" t="n">
         <v>8.674877</v>
       </c>
-      <c r="F16" t="n">
+      <c r="F16" s="0" t="n">
         <v>50.586195</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" s="0" t="n">
         <v>271667</v>
       </c>
-      <c r="H16" t="s">
+      <c r="H16" s="0" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="E17" t="n">
+      <c r="E17" s="0" t="n">
         <v>8.501069</v>
       </c>
-      <c r="F17" t="n">
+      <c r="F17" s="0" t="n">
         <v>50.554439</v>
       </c>
-      <c r="G17" t="n">
+      <c r="G17" s="0" t="n">
         <v>253373</v>
       </c>
-      <c r="H17" t="s">
+      <c r="H17" s="0" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
         <v>72</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="0" t="s">
         <v>74</v>
       </c>
-      <c r="E18" t="n">
+      <c r="E18" s="0" t="n">
         <v>8.064098</v>
       </c>
-      <c r="F18" t="n">
+      <c r="F18" s="0" t="n">
         <v>50.387254</v>
       </c>
-      <c r="G18" t="n">
+      <c r="G18" s="0" t="n">
         <v>172291</v>
       </c>
-      <c r="H18" t="s">
+      <c r="H18" s="0" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19">
-      <c r="A19" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
         <v>76</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="0" t="s">
         <v>77</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="E19" t="n">
+      <c r="E19" s="0" t="n">
         <v>8.769147</v>
       </c>
-      <c r="F19" t="n">
+      <c r="F19" s="0" t="n">
         <v>50.809004</v>
       </c>
-      <c r="G19" t="n">
+      <c r="G19" s="0" t="n">
         <v>245903</v>
       </c>
-      <c r="H19" t="s">
+      <c r="H19" s="0" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20" s="0" t="n">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="0" t="s">
         <v>81</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="E20" t="n">
+      <c r="E20" s="0" t="n">
         <v>9.397967</v>
       </c>
-      <c r="F20" t="n">
+      <c r="F20" s="0" t="n">
         <v>50.635729</v>
       </c>
-      <c r="G20" t="n">
+      <c r="G20" s="0" t="n">
         <v>105506</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H20" s="0" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21">
-      <c r="A21" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="0" t="s">
         <v>85</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="0" t="s">
         <v>86</v>
       </c>
-      <c r="E21" t="n">
+      <c r="E21" s="0" t="n">
         <v>9.495199</v>
       </c>
-      <c r="F21" t="n">
+      <c r="F21" s="0" t="n">
         <v>51.314684</v>
       </c>
-      <c r="G21" t="n">
+      <c r="G21" s="0" t="n">
         <v>201048</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H21" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22">
-      <c r="A22" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E22" s="0" t="n">
         <v>9.675061</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F22" s="0" t="n">
         <v>50.55323</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G22" s="0" t="n">
         <v>223023</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H22" s="0" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23">
-      <c r="A23" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="E23" t="n">
+      <c r="E23" s="0" t="n">
         <v>9.706008</v>
       </c>
-      <c r="F23" t="n">
+      <c r="F23" s="0" t="n">
         <v>50.867805</v>
       </c>
-      <c r="G23" t="n">
+      <c r="G23" s="0" t="n">
         <v>120304</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H23" s="0" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="0" t="s">
         <v>97</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="E24" t="n">
+      <c r="E24" s="0" t="n">
         <v>9.383496</v>
       </c>
-      <c r="F24" t="n">
+      <c r="F24" s="0" t="n">
         <v>51.494179</v>
       </c>
-      <c r="G24" t="n">
+      <c r="G24" s="0" t="n">
         <v>237007</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H24" s="0" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25">
-      <c r="A25" t="s">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25" s="0" t="n">
         <v>21</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="E25" t="n">
+      <c r="E25" s="0" t="n">
         <v>9.275373</v>
       </c>
-      <c r="F25" t="n">
+      <c r="F25" s="0" t="n">
         <v>51.13094</v>
       </c>
-      <c r="G25" t="n">
+      <c r="G25" s="0" t="n">
         <v>179840</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="0" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="26">
-      <c r="A26" t="s">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26" s="0" t="n">
         <v>23</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="0" t="s">
         <v>104</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="E26" t="n">
+      <c r="E26" s="0" t="n">
         <v>8.873194</v>
       </c>
-      <c r="F26" t="n">
+      <c r="F26" s="0" t="n">
         <v>51.27186</v>
       </c>
-      <c r="G26" t="n">
+      <c r="G26" s="0" t="n">
         <v>156528</v>
       </c>
-      <c r="H26" t="s">
+      <c r="H26" s="0" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27" t="s">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27" s="0" t="n">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="E27" t="n">
+      <c r="E27" s="0" t="n">
         <v>10.057981</v>
       </c>
-      <c r="F27" t="n">
+      <c r="F27" s="0" t="n">
         <v>51.185804</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27" s="0" t="n">
         <v>100046</v>
       </c>
-      <c r="H27" t="s">
+      <c r="H27" s="0" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <hyperlinks>
+    <hyperlink ref="H8" r:id="rId1" display="https://www.kreisgg.de/gesundheit/"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Neue Datenquelle: Todesfälle nach Sterbedatum
</commit_message>
<xml_diff>
--- a/index/kreise-index-pop.xlsx
+++ b/index/kreise-index-pop.xlsx
@@ -103,7 +103,7 @@
     <t xml:space="preserve">Heppenheim (Bergstraße), Kreisstadt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.kreis-bergstrasse.de/staticsite/staticsite.php?menuid=613&amp;topmenu=467</t>
+    <t xml:space="preserve">https://www.kreis-bergstrasse.de/aktuelles-veroeffentlichungen/corona/</t>
   </si>
   <si>
     <t xml:space="preserve">Darmstadt-Dieburg</t>
@@ -428,8 +428,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -453,716 +457,716 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>8.653838</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>49.872238</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>159174</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>8.682433</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>50.11088</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>764104</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>8.784442</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>50.100567</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>130892</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="H4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="1" t="n">
         <v>8.239138</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <v>50.081698</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="G5" s="1" t="n">
         <v>278609</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="1" t="n">
         <v>8.644017</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <v>49.641185</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="G6" s="1" t="n">
         <v>271015</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="1" t="n">
         <v>8.840041</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <v>49.899272</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="G7" s="1" t="n">
         <v>297701</v>
       </c>
-      <c r="H7" s="0" t="s">
+      <c r="H7" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="1" t="n">
         <v>8.482423</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <v>49.92162</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="G8" s="1" t="n">
         <v>275807</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="1" t="n">
         <v>8.61299</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <v>50.228406</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>237281</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="H9" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="1" t="n">
         <v>9.191488</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="1" t="n">
         <v>50.203103</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>421689</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="H10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="1" t="n">
         <v>8.446053</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="1" t="n">
         <v>50.088576</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="G11" s="1" t="n">
         <v>239264</v>
       </c>
-      <c r="H11" s="0" t="s">
+      <c r="H11" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="1" t="n">
         <v>8.99268</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <v>49.657653</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="G12" s="1" t="n">
         <v>96754</v>
       </c>
-      <c r="H12" s="0" t="s">
+      <c r="H12" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="1" t="n">
         <v>8.781779</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <v>50.008939</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="G13" s="1" t="n">
         <v>356542</v>
       </c>
-      <c r="H13" s="0" t="s">
+      <c r="H13" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="1" t="n">
         <v>8.069825</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <v>50.140276</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="G14" s="1" t="n">
         <v>187433</v>
       </c>
-      <c r="H14" s="0" t="s">
+      <c r="H14" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="0" t="n">
+      <c r="B15" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="1" t="n">
         <v>8.754091</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <v>50.33776</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="G15" s="1" t="n">
         <v>310353</v>
       </c>
-      <c r="H15" s="0" t="s">
+      <c r="H15" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="0" t="n">
+      <c r="B16" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="1" t="n">
         <v>8.674877</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <v>50.586195</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="G16" s="1" t="n">
         <v>271667</v>
       </c>
-      <c r="H16" s="0" t="s">
+      <c r="H16" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="0" t="n">
+      <c r="B17" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="1" t="n">
         <v>8.501069</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="1" t="n">
         <v>50.554439</v>
       </c>
-      <c r="G17" s="0" t="n">
+      <c r="G17" s="1" t="n">
         <v>253373</v>
       </c>
-      <c r="H17" s="0" t="s">
+      <c r="H17" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="0" t="n">
+      <c r="B18" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="1" t="n">
         <v>8.064098</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="1" t="n">
         <v>50.387254</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="G18" s="1" t="n">
         <v>172291</v>
       </c>
-      <c r="H18" s="0" t="s">
+      <c r="H18" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="0" t="n">
+      <c r="B19" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="1" t="n">
         <v>8.769147</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="1" t="n">
         <v>50.809004</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="G19" s="1" t="n">
         <v>245903</v>
       </c>
-      <c r="H19" s="0" t="s">
+      <c r="H19" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="0" t="n">
+      <c r="B20" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="1" t="n">
         <v>9.397967</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="1" t="n">
         <v>50.635729</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="G20" s="1" t="n">
         <v>105506</v>
       </c>
-      <c r="H20" s="0" t="s">
+      <c r="H20" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="0" t="n">
+      <c r="B21" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="0" t="n">
+      <c r="E21" s="1" t="n">
         <v>9.495199</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="1" t="n">
         <v>51.314684</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="G21" s="1" t="n">
         <v>201048</v>
       </c>
-      <c r="H21" s="0" t="s">
+      <c r="H21" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="0" t="n">
+      <c r="B22" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="0" t="n">
+      <c r="E22" s="1" t="n">
         <v>9.675061</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="1" t="n">
         <v>50.55323</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="G22" s="1" t="n">
         <v>223023</v>
       </c>
-      <c r="H22" s="0" t="s">
+      <c r="H22" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="0" t="n">
+      <c r="B23" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="0" t="n">
+      <c r="E23" s="1" t="n">
         <v>9.706008</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="1" t="n">
         <v>50.867805</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="G23" s="1" t="n">
         <v>120304</v>
       </c>
-      <c r="H23" s="0" t="s">
+      <c r="H23" s="1" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="0" t="n">
+      <c r="B24" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="0" t="n">
+      <c r="E24" s="1" t="n">
         <v>9.383496</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="1" t="n">
         <v>51.494179</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="G24" s="1" t="n">
         <v>237007</v>
       </c>
-      <c r="H24" s="0" t="s">
+      <c r="H24" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="0" t="n">
+      <c r="B25" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="0" t="s">
+      <c r="D25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="0" t="n">
+      <c r="E25" s="1" t="n">
         <v>9.275373</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="1" t="n">
         <v>51.13094</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="G25" s="1" t="n">
         <v>179840</v>
       </c>
-      <c r="H25" s="0" t="s">
+      <c r="H25" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="0" t="n">
+      <c r="B26" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="0" t="s">
+      <c r="D26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="1" t="n">
         <v>8.873194</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="1" t="n">
         <v>51.27186</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="G26" s="1" t="n">
         <v>156528</v>
       </c>
-      <c r="H26" s="0" t="s">
+      <c r="H26" s="1" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="0" t="n">
+      <c r="B27" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="0" t="s">
+      <c r="D27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="1" t="n">
         <v>10.057981</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="1" t="n">
         <v>51.185804</v>
       </c>
-      <c r="G27" s="0" t="n">
+      <c r="G27" s="1" t="n">
         <v>100046</v>
       </c>
-      <c r="H27" s="0" t="s">
+      <c r="H27" s="1" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" display="https://www.kreisgg.de/gesundheit/"/>
+    <hyperlink ref="H8" r:id="rId1" display="https://www.kreisgg.de/gesundheit/corona-krise-info-und-hotlines/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
Anpassung an neue Bevölkerungszahlen Stand 12/2021, neue RKI-Repo-Struktur
</commit_message>
<xml_diff>
--- a/index/kreise-index-pop.xlsx
+++ b/index/kreise-index-pop.xlsx
@@ -1,26 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t xml:space="preserve">kreis</t>
   </si>
@@ -259,7 +251,7 @@
     <t xml:space="preserve">Marburg, Universitätsstadt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.marburg-biedenkopf.de/soziales_und_gesundheit/corona/Aktuelle-Corona-Zahlen.php</t>
+    <t xml:space="preserve">https://corona.marburg-biedenkopf.de/Aktuelle_Zahlen___Regelungen/inhalte-aktuelle-zahlen/Aktuelle-Corona-Zahlen.php</t>
   </si>
   <si>
     <t xml:space="preserve">Vogelsbergkreis</t>
@@ -328,7 +320,7 @@
     <t xml:space="preserve">Fritzlar, Dom- und Kaiserstadt</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.schwalm-eder-kreis.de/Aktuelles/Aktuelle-Informationen-zum-neuartigen-Coronavirus-Covid-19/Aktuelle-Zahlen-Schwalm-Eder.htm?</t>
+    <t xml:space="preserve">https://www.schwalm-eder-kreis.de/Home.htm?</t>
   </si>
   <si>
     <t xml:space="preserve">Waldeck-Frankenberg</t>
@@ -358,32 +350,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -395,7 +370,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -403,777 +378,1008 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H20" activeCellId="0" sqref="H20"/>
-    </sheetView>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2">
+      <c r="A2" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" t="n">
         <v>2</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="1" t="n">
+      <c r="E2" t="n">
         <v>8.653838</v>
       </c>
-      <c r="F2" s="1" t="n">
+      <c r="F2" t="n">
         <v>49.872238</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <v>159174</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="G2" t="n">
+        <v>159631</v>
+      </c>
+      <c r="H2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" t="n">
         <v>4</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1" t="n">
+      <c r="E3" t="n">
         <v>8.682433</v>
       </c>
-      <c r="F3" s="1" t="n">
+      <c r="F3" t="n">
         <v>50.11088</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <v>764104</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="G3" t="n">
+        <v>759224</v>
+      </c>
+      <c r="H3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" t="n">
         <v>19</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="n">
+      <c r="E4" t="n">
         <v>8.784442</v>
       </c>
-      <c r="F4" s="1" t="n">
+      <c r="F4" t="n">
         <v>50.100567</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <v>130892</v>
-      </c>
-      <c r="H4" s="1" t="s">
+      <c r="G4" t="n">
+        <v>131295</v>
+      </c>
+      <c r="H4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+    <row r="5">
+      <c r="A5" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" t="n">
         <v>26</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="1" t="n">
+      <c r="E5" t="n">
         <v>8.239138</v>
       </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" t="n">
         <v>50.081698</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <v>278609</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="G5" t="n">
+        <v>278950</v>
+      </c>
+      <c r="H5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+    <row r="6">
+      <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="1" t="n">
+      <c r="B6" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" t="n">
         <v>8.644017</v>
       </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" t="n">
         <v>49.641185</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <v>271015</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="G6" t="n">
+        <v>271166</v>
+      </c>
+      <c r="H6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+    <row r="7">
+      <c r="A7" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="1" t="n">
+      <c r="B7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>30</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" t="n">
         <v>8.840041</v>
       </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" t="n">
         <v>49.899272</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <v>297701</v>
-      </c>
-      <c r="H7" s="1" t="s">
+      <c r="G7" t="n">
+        <v>296900</v>
+      </c>
+      <c r="H7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+    <row r="8">
+      <c r="A8" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" t="n">
         <v>7</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>34</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" t="n">
         <v>8.482423</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="F8" t="n">
         <v>49.92162</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <v>275807</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="G8" t="n">
+        <v>276307</v>
+      </c>
+      <c r="H8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="9">
+      <c r="A9" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="1" t="n">
+      <c r="B9" t="n">
         <v>9</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" t="n">
         <v>8.61299</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="F9" t="n">
         <v>50.228406</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <v>237281</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="G9" t="n">
+        <v>237041</v>
+      </c>
+      <c r="H9" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
+    <row r="10">
+      <c r="A10" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="1" t="n">
+      <c r="B10" t="n">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" t="n">
         <v>9.191488</v>
       </c>
-      <c r="F10" s="1" t="n">
+      <c r="F10" t="n">
         <v>50.203103</v>
       </c>
-      <c r="G10" s="1" t="n">
-        <v>421689</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="G10" t="n">
+        <v>423465</v>
+      </c>
+      <c r="H10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
+    <row r="11">
+      <c r="A11" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" t="n">
         <v>15</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" t="n">
         <v>8.446053</v>
       </c>
-      <c r="F11" s="1" t="n">
+      <c r="F11" t="n">
         <v>50.088576</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <v>239264</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="G11" t="n">
+        <v>239276</v>
+      </c>
+      <c r="H11" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
+    <row r="12">
+      <c r="A12" t="s">
         <v>48</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" t="n">
         <v>17</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>49</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>50</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" t="n">
         <v>8.99268</v>
       </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" t="n">
         <v>49.657653</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <v>96754</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="G12" t="n">
+        <v>96953</v>
+      </c>
+      <c r="H12" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+    <row r="13">
+      <c r="A13" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="1" t="n">
+      <c r="B13" t="n">
         <v>18</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>54</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" t="n">
         <v>8.781779</v>
       </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" t="n">
         <v>50.008939</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <v>356542</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="G13" t="n">
+        <v>357466</v>
+      </c>
+      <c r="H13" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+    <row r="14">
+      <c r="A14" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" t="n">
         <v>20</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>57</v>
       </c>
-      <c r="D14" s="1" t="s">
+      <c r="D14" t="s">
         <v>58</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" t="n">
         <v>8.069825</v>
       </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" t="n">
         <v>50.140276</v>
       </c>
-      <c r="G14" s="1" t="n">
-        <v>187433</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="G14" t="n">
+        <v>187229</v>
+      </c>
+      <c r="H14" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
+    <row r="15">
+      <c r="A15" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="1" t="n">
+      <c r="B15" t="n">
         <v>25</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>61</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" t="n">
         <v>8.754091</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="F15" t="n">
         <v>50.33776</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <v>310353</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="G15" t="n">
+        <v>311661</v>
+      </c>
+      <c r="H15" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
+    <row r="16">
+      <c r="A16" t="s">
         <v>64</v>
       </c>
-      <c r="B16" s="1" t="n">
+      <c r="B16" t="n">
         <v>6</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>65</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" t="n">
         <v>8.674877</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="F16" t="n">
         <v>50.586195</v>
       </c>
-      <c r="G16" s="1" t="n">
-        <v>271667</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="G16" t="n">
+        <v>272874</v>
+      </c>
+      <c r="H16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+    <row r="17">
+      <c r="A17" t="s">
         <v>68</v>
       </c>
-      <c r="B17" s="1" t="n">
+      <c r="B17" t="n">
         <v>12</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" t="n">
         <v>8.501069</v>
       </c>
-      <c r="F17" s="1" t="n">
+      <c r="F17" t="n">
         <v>50.554439</v>
       </c>
-      <c r="G17" s="1" t="n">
-        <v>253373</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="G17" t="n">
+        <v>253364</v>
+      </c>
+      <c r="H17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="18">
+      <c r="A18" t="s">
         <v>72</v>
       </c>
-      <c r="B18" s="1" t="n">
+      <c r="B18" t="n">
         <v>13</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" t="n">
         <v>8.064098</v>
       </c>
-      <c r="F18" s="1" t="n">
+      <c r="F18" t="n">
         <v>50.387254</v>
       </c>
-      <c r="G18" s="1" t="n">
-        <v>172291</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="G18" t="n">
+        <v>172759</v>
+      </c>
+      <c r="H18" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="19">
+      <c r="A19" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="1" t="n">
+      <c r="B19" t="n">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" t="n">
         <v>8.769147</v>
       </c>
-      <c r="F19" s="1" t="n">
+      <c r="F19" t="n">
         <v>50.809004</v>
       </c>
-      <c r="G19" s="1" t="n">
-        <v>245903</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="G19" t="n">
+        <v>246097</v>
+      </c>
+      <c r="H19" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1" t="s">
+    <row r="20">
+      <c r="A20" t="s">
         <v>80</v>
       </c>
-      <c r="B20" s="1" t="n">
+      <c r="B20" t="n">
         <v>22</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>81</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
         <v>82</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" t="n">
         <v>9.397967</v>
       </c>
-      <c r="F20" s="1" t="n">
+      <c r="F20" t="n">
         <v>50.635729</v>
       </c>
-      <c r="G20" s="1" t="n">
-        <v>105506</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="G20" t="n">
+        <v>105671</v>
+      </c>
+      <c r="H20" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1" t="s">
+    <row r="21">
+      <c r="A21" t="s">
         <v>84</v>
       </c>
-      <c r="B21" s="1" t="n">
+      <c r="B21" t="n">
         <v>11</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" t="s">
         <v>85</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="D21" t="s">
         <v>86</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" t="n">
         <v>9.495199</v>
       </c>
-      <c r="F21" s="1" t="n">
+      <c r="F21" t="n">
         <v>51.314684</v>
       </c>
-      <c r="G21" s="1" t="n">
-        <v>201048</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="G21" t="n">
+        <v>200406</v>
+      </c>
+      <c r="H21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1" t="s">
+    <row r="22">
+      <c r="A22" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="1" t="n">
+      <c r="B22" t="n">
         <v>5</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C22" t="s">
         <v>89</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D22" t="s">
         <v>90</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" t="n">
         <v>9.675061</v>
       </c>
-      <c r="F22" s="1" t="n">
+      <c r="F22" t="n">
         <v>50.55323</v>
       </c>
-      <c r="G22" s="1" t="n">
-        <v>223023</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="G22" t="n">
+        <v>223572</v>
+      </c>
+      <c r="H22" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
+    <row r="23">
+      <c r="A23" t="s">
         <v>92</v>
       </c>
-      <c r="B23" s="1" t="n">
+      <c r="B23" t="n">
         <v>8</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" t="s">
         <v>93</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="D23" t="s">
         <v>94</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" t="n">
         <v>9.706008</v>
       </c>
-      <c r="F23" s="1" t="n">
+      <c r="F23" t="n">
         <v>50.867805</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <v>120304</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="G23" t="n">
+        <v>120163</v>
+      </c>
+      <c r="H23" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1" t="s">
+    <row r="24">
+      <c r="A24" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="1" t="n">
+      <c r="B24" t="n">
         <v>10</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="D24" t="s">
         <v>98</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" t="n">
         <v>9.383496</v>
       </c>
-      <c r="F24" s="1" t="n">
+      <c r="F24" t="n">
         <v>51.494179</v>
       </c>
-      <c r="G24" s="1" t="n">
-        <v>237007</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="G24" t="n">
+        <v>237268</v>
+      </c>
+      <c r="H24" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+    <row r="25">
+      <c r="A25" t="s">
         <v>99</v>
       </c>
-      <c r="B25" s="1" t="n">
+      <c r="B25" t="n">
         <v>21</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D25" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" t="n">
         <v>9.275373</v>
       </c>
-      <c r="F25" s="1" t="n">
+      <c r="F25" t="n">
         <v>51.13094</v>
       </c>
-      <c r="G25" s="1" t="n">
-        <v>179840</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="G25" t="n">
+        <v>180052</v>
+      </c>
+      <c r="H25" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
+    <row r="26">
+      <c r="A26" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="1" t="n">
+      <c r="B26" t="n">
         <v>23</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" t="s">
         <v>104</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D26" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" t="n">
         <v>8.873194</v>
       </c>
-      <c r="F26" s="1" t="n">
+      <c r="F26" t="n">
         <v>51.27186</v>
       </c>
-      <c r="G26" s="1" t="n">
-        <v>156528</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="G26" t="n">
+        <v>156513</v>
+      </c>
+      <c r="H26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
+    <row r="27">
+      <c r="A27" t="s">
         <v>107</v>
       </c>
-      <c r="B27" s="1" t="n">
+      <c r="B27" t="n">
         <v>24</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" t="s">
         <v>108</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" t="n">
         <v>10.057981</v>
       </c>
-      <c r="F27" s="1" t="n">
+      <c r="F27" t="n">
         <v>51.185804</v>
       </c>
-      <c r="G27" s="1" t="n">
-        <v>100046</v>
-      </c>
-      <c r="H27" s="1" t="s">
+      <c r="G27" t="n">
+        <v>99714</v>
+      </c>
+      <c r="H27" t="s">
         <v>110</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="H8" r:id="rId1" display="https://www.kreisgg.de/gesundheit/corona-krise-info-und-hotlines/"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>